<commit_message>
Added test run for 5/7/2020
</commit_message>
<xml_diff>
--- a/Project.xlsx
+++ b/Project.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shavk\Repos\github.com\aynurin\fin-forecast\webapp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9A79600-0856-4BF4-8AD4-59959B90EEB0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA082248-4A74-4070-AE06-C15C82AB060B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10546" activeTab="1" xr2:uid="{66BD318F-A7B9-4F37-B102-2FA1278077E0}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="425" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="488" uniqueCount="100">
   <si>
     <t>Adjust account totals</t>
   </si>
@@ -1413,10 +1413,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D412D44-9E6C-4E88-9D45-D1CA2BD14B37}">
-  <dimension ref="A1:G64"/>
+  <dimension ref="A1:H64"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1425,7 +1425,7 @@
     <col min="5" max="7" width="9.19921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
         <v>41</v>
@@ -1445,8 +1445,11 @@
       <c r="G1" s="3">
         <v>43951</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H1" s="3">
+        <v>43958</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A2" s="4" t="s">
         <v>42</v>
       </c>
@@ -1468,8 +1471,11 @@
       <c r="G2" s="1" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H2" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A3" s="1"/>
       <c r="B3" s="6" t="s">
         <v>45</v>
@@ -1489,8 +1495,11 @@
       <c r="G3" s="1" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H3" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A4" s="1"/>
       <c r="B4" s="6" t="s">
         <v>46</v>
@@ -1510,8 +1519,11 @@
       <c r="G4" s="1" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" ht="71.25" x14ac:dyDescent="0.45">
+      <c r="H4" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A5" s="4" t="s">
         <v>47</v>
       </c>
@@ -1533,8 +1545,11 @@
       <c r="G5" s="1" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H5" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A6" s="1"/>
       <c r="B6" s="6" t="s">
         <v>49</v>
@@ -1554,8 +1569,11 @@
       <c r="G6" s="1" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H6" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A7" s="1"/>
       <c r="B7" s="6" t="s">
         <v>50</v>
@@ -1571,8 +1589,11 @@
       <c r="G7" s="1" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H7" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A8" s="1"/>
       <c r="B8" s="6" t="s">
         <v>90</v>
@@ -1588,8 +1609,11 @@
       <c r="G8" s="1" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H8" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A9" s="1"/>
       <c r="B9" s="6" t="s">
         <v>91</v>
@@ -1609,8 +1633,11 @@
       <c r="G9" s="1" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H9" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A10" s="1"/>
       <c r="B10" s="6" t="s">
         <v>53</v>
@@ -1630,8 +1657,11 @@
       <c r="G10" s="1" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H10" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A11" s="1"/>
       <c r="B11" s="6" t="s">
         <v>54</v>
@@ -1651,8 +1681,11 @@
       <c r="G11" s="1" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H11" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A12" s="1"/>
       <c r="B12" s="6" t="s">
         <v>55</v>
@@ -1672,8 +1705,11 @@
       <c r="G12" s="1" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H12" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A13" s="1"/>
       <c r="B13" s="6" t="s">
         <v>57</v>
@@ -1693,8 +1729,11 @@
       <c r="G13" s="1" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H13" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A14" s="1"/>
       <c r="B14" s="6" t="s">
         <v>58</v>
@@ -1714,8 +1753,11 @@
       <c r="G14" s="1" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H14" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A15" s="1"/>
       <c r="B15" s="6" t="s">
         <v>59</v>
@@ -1735,8 +1777,11 @@
       <c r="G15" s="1" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H15" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A16" s="1"/>
       <c r="B16" s="6" t="s">
         <v>92</v>
@@ -1750,8 +1795,11 @@
       <c r="G16" s="1" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H16" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A17" s="1"/>
       <c r="B17" s="6" t="s">
         <v>93</v>
@@ -1765,8 +1813,11 @@
       <c r="G17" s="1" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="H17" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A18" s="4" t="s">
         <v>60</v>
       </c>
@@ -1786,8 +1837,11 @@
       <c r="G18" s="1" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H18" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A19" s="1"/>
       <c r="B19" s="6" t="s">
         <v>94</v>
@@ -1805,8 +1859,11 @@
       <c r="G19" s="1" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H19" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A20" s="1"/>
       <c r="B20" s="6" t="s">
         <v>62</v>
@@ -1824,8 +1881,11 @@
       <c r="G20" s="1" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H20" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A21" s="1"/>
       <c r="B21" s="6" t="s">
         <v>63</v>
@@ -1843,8 +1903,11 @@
       <c r="G21" s="1" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H21" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A22" s="1"/>
       <c r="B22" s="6" t="s">
         <v>55</v>
@@ -1862,8 +1925,11 @@
       <c r="G22" s="1" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H22" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A23" s="1"/>
       <c r="B23" s="6" t="s">
         <v>64</v>
@@ -1881,8 +1947,11 @@
       <c r="G23" s="1" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H23" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A24" s="1"/>
       <c r="B24" s="6" t="s">
         <v>65</v>
@@ -1900,8 +1969,11 @@
       <c r="G24" s="1" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H24" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A25" s="1"/>
       <c r="B25" s="6" t="s">
         <v>66</v>
@@ -1919,8 +1991,11 @@
       <c r="G25" s="1" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H25" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A26" s="1"/>
       <c r="B26" s="6" t="s">
         <v>92</v>
@@ -1934,8 +2009,11 @@
       <c r="G26" s="1" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H26" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A27" s="1"/>
       <c r="B27" s="6" t="s">
         <v>93</v>
@@ -1949,8 +2027,11 @@
       <c r="G27" s="1" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" ht="57" x14ac:dyDescent="0.45">
+      <c r="H27" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="57" x14ac:dyDescent="0.45">
       <c r="A28" s="4" t="s">
         <v>67</v>
       </c>
@@ -1970,8 +2051,11 @@
       <c r="G28" s="1" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H28" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A29" s="1"/>
       <c r="B29" s="6" t="s">
         <v>51</v>
@@ -1989,8 +2073,11 @@
       <c r="G29" s="1" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H29" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A30" s="1"/>
       <c r="B30" s="6" t="s">
         <v>69</v>
@@ -2008,8 +2095,11 @@
       <c r="G30" s="1" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H30" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A31" s="1"/>
       <c r="B31" s="6" t="s">
         <v>70</v>
@@ -2027,8 +2117,11 @@
       <c r="G31" s="1" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H31" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A32" s="1"/>
       <c r="B32" s="6" t="s">
         <v>55</v>
@@ -2046,8 +2139,11 @@
       <c r="G32" s="1" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H32" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A33" s="1"/>
       <c r="B33" s="6" t="s">
         <v>71</v>
@@ -2065,8 +2161,11 @@
       <c r="G33" s="1" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H33" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A34" s="1"/>
       <c r="B34" s="6" t="s">
         <v>72</v>
@@ -2084,8 +2183,11 @@
       <c r="G34" s="1" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H34" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A35" s="1"/>
       <c r="B35" s="6" t="s">
         <v>92</v>
@@ -2099,8 +2201,11 @@
       <c r="G35" s="1" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H35" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A36" s="1"/>
       <c r="B36" s="6" t="s">
         <v>93</v>
@@ -2114,8 +2219,11 @@
       <c r="G36" s="1" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="37" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="H36" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A37" s="4" t="s">
         <v>98</v>
       </c>
@@ -2135,8 +2243,11 @@
       <c r="G37" s="1" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H37" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A38" s="1"/>
       <c r="B38" s="6" t="s">
         <v>73</v>
@@ -2154,8 +2265,11 @@
       <c r="G38" s="1" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H38" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A39" s="1"/>
       <c r="B39" s="6" t="s">
         <v>74</v>
@@ -2173,8 +2287,11 @@
       <c r="G39" s="1" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H39" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A40" s="1"/>
       <c r="B40" s="6" t="s">
         <v>92</v>
@@ -2188,8 +2305,11 @@
       <c r="G40" s="1" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H40" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A41" s="1"/>
       <c r="B41" s="6" t="s">
         <v>93</v>
@@ -2203,8 +2323,11 @@
       <c r="G41" s="1" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="42" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="H41" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A42" s="4" t="s">
         <v>75</v>
       </c>
@@ -2222,8 +2345,11 @@
       <c r="G42" s="1" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H42" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A43" s="1"/>
       <c r="B43" s="6" t="s">
         <v>76</v>
@@ -2239,8 +2365,11 @@
       <c r="G43" s="1" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="44" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="H43" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A44" s="1"/>
       <c r="B44" s="6" t="s">
         <v>77</v>
@@ -2256,8 +2385,11 @@
       <c r="G44" s="1" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H44" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A45" s="1"/>
       <c r="B45" s="6" t="s">
         <v>78</v>
@@ -2273,8 +2405,11 @@
       <c r="G45" s="1" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H45" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.45">
       <c r="B46" s="6" t="s">
         <v>79</v>
       </c>
@@ -2287,8 +2422,11 @@
       <c r="G46" s="1" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="47" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="H46" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B47" s="6" t="s">
         <v>77</v>
       </c>
@@ -2301,8 +2439,11 @@
       <c r="G47" s="1" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H47" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.45">
       <c r="B48" s="6" t="s">
         <v>80</v>
       </c>
@@ -2315,8 +2456,11 @@
       <c r="G48" s="1" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H48" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.45">
       <c r="B49" s="6" t="s">
         <v>79</v>
       </c>
@@ -2329,8 +2473,11 @@
       <c r="G49" s="1" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H49" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.45">
       <c r="B50" s="6" t="s">
         <v>81</v>
       </c>
@@ -2343,8 +2490,11 @@
       <c r="G50" s="1" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H50" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.45">
       <c r="B51" s="6" t="s">
         <v>76</v>
       </c>
@@ -2357,8 +2507,11 @@
       <c r="G51" s="1" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H51" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.45">
       <c r="B52" s="6" t="s">
         <v>81</v>
       </c>
@@ -2371,8 +2524,11 @@
       <c r="G52" s="1" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="53" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="H52" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A53" s="4" t="s">
         <v>82</v>
       </c>
@@ -2388,8 +2544,11 @@
       <c r="G53" s="1" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H53" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A54" s="1"/>
       <c r="B54" s="6" t="s">
         <v>85</v>
@@ -2403,8 +2562,11 @@
       <c r="G54" s="1" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H54" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A55" s="1"/>
       <c r="B55" s="6" t="s">
         <v>86</v>
@@ -2418,8 +2580,11 @@
       <c r="G55" s="1" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H55" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A56" s="1"/>
       <c r="B56" s="6" t="s">
         <v>87</v>
@@ -2433,8 +2598,11 @@
       <c r="G56" s="1" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H56" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.45">
       <c r="B57" s="6" t="s">
         <v>88</v>
       </c>
@@ -2445,8 +2613,11 @@
       <c r="G57" s="1" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H57" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.45">
       <c r="B58" s="6" t="s">
         <v>89</v>
       </c>
@@ -2457,8 +2628,11 @@
       <c r="G58" s="1" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H58" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.45">
       <c r="B59" s="6" t="s">
         <v>81</v>
       </c>
@@ -2469,8 +2643,11 @@
       <c r="G59" s="1" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H59" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.45">
       <c r="B60" s="6" t="s">
         <v>85</v>
       </c>
@@ -2481,8 +2658,11 @@
       <c r="G60" s="1" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H60" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.45">
       <c r="B61" s="6" t="s">
         <v>81</v>
       </c>
@@ -2493,8 +2673,11 @@
       <c r="G61" s="1" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H61" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.45">
       <c r="B62" s="6" t="s">
         <v>95</v>
       </c>
@@ -2505,8 +2688,11 @@
       <c r="G62" s="1" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="63" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="H62" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B63" s="6" t="s">
         <v>96</v>
       </c>
@@ -2517,8 +2703,11 @@
       <c r="G63" s="1" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H63" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.45">
       <c r="B64" s="6" t="s">
         <v>97</v>
       </c>
@@ -2526,6 +2715,9 @@
         <v>44</v>
       </c>
       <c r="G64" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="H64" s="1" t="s">
         <v>44</v>
       </c>
     </row>

</xml_diff>